<commit_message>
feat: show enum answers distribution, better logging, App.reload
</commit_message>
<xml_diff>
--- a/data/post/YTC.xlsx
+++ b/data/post/YTC.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3359" uniqueCount="703">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3359" uniqueCount="702">
   <si>
     <t xml:space="preserve">Column 43</t>
   </si>
@@ -575,7 +575,7 @@
     <t xml:space="preserve">johnadalbert206@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">John Adalbert 206@gmail.com</t>
+    <t xml:space="preserve">John Adalbert</t>
   </si>
   <si>
     <t xml:space="preserve">depuis moins des octobre 2025</t>
@@ -1788,9 +1788,6 @@
   </si>
   <si>
     <t xml:space="preserve">I appreciate the opportunity given to me </t>
-  </si>
-  <si>
-    <t xml:space="preserve">johnadalbert206@gmail.com g</t>
   </si>
   <si>
     <t xml:space="preserve">Pas difficile </t>
@@ -2646,14 +2643,16 @@
   <dimension ref="A1:AW1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="E62" activeCellId="0" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="6" style="1" width="37.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="44" style="1" width="18.88"/>
   </cols>
@@ -10274,7 +10273,7 @@
         <v>181</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>572</v>
+        <v>181</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>186</v>
@@ -10358,13 +10357,13 @@
         <v>106</v>
       </c>
       <c r="AG59" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="AH59" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="AI59" s="9" t="s">
         <v>573</v>
-      </c>
-      <c r="AH59" s="9" t="s">
-        <v>573</v>
-      </c>
-      <c r="AI59" s="9" t="s">
-        <v>574</v>
       </c>
       <c r="AJ59" s="9" t="s">
         <v>190</v>
@@ -10373,7 +10372,7 @@
         <v>190</v>
       </c>
       <c r="AL59" s="9" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="AM59" s="9" t="s">
         <v>95</v>
@@ -10405,7 +10404,7 @@
         <v>326</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>146</v>
@@ -10420,7 +10419,7 @@
         <v>185</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K60" s="9" t="s">
         <v>120</v>
@@ -10498,10 +10497,10 @@
         <v>491</v>
       </c>
       <c r="AJ60" s="9" t="s">
+        <v>577</v>
+      </c>
+      <c r="AK60" s="9" t="s">
         <v>578</v>
-      </c>
-      <c r="AK60" s="9" t="s">
-        <v>579</v>
       </c>
       <c r="AL60" s="9" t="s">
         <v>333</v>
@@ -10516,7 +10515,7 @@
         <v>142</v>
       </c>
       <c r="AP60" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="AQ60" s="9" t="s">
         <v>212</v>
@@ -10533,10 +10532,10 @@
         <v>46034.4198070718</v>
       </c>
       <c r="D61" s="9" t="s">
+        <v>580</v>
+      </c>
+      <c r="E61" s="9" t="s">
         <v>581</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>582</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>146</v>
@@ -10551,7 +10550,7 @@
         <v>103</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="K61" s="9" t="s">
         <v>106</v>
@@ -10626,10 +10625,10 @@
         <v>470</v>
       </c>
       <c r="AI61" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="AJ61" s="9" t="s">
         <v>584</v>
-      </c>
-      <c r="AJ61" s="9" t="s">
-        <v>585</v>
       </c>
       <c r="AK61" s="9" t="s">
         <v>345</v>
@@ -10647,7 +10646,7 @@
         <v>97</v>
       </c>
       <c r="AP61" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="AQ61" s="9" t="s">
         <v>345</v>
@@ -10664,10 +10663,10 @@
         <v>46034.4212326273</v>
       </c>
       <c r="D62" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="E62" s="9" t="s">
         <v>587</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>588</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>545</v>
@@ -10682,7 +10681,7 @@
         <v>185</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K62" s="9" t="s">
         <v>106</v>
@@ -10763,7 +10762,7 @@
         <v>153</v>
       </c>
       <c r="AK62" s="9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="AL62" s="9" t="s">
         <v>384</v>
@@ -10772,7 +10771,7 @@
         <v>95</v>
       </c>
       <c r="AN62" s="9" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="AO62" s="9" t="s">
         <v>169</v>
@@ -10882,13 +10881,13 @@
         <v>106</v>
       </c>
       <c r="AG63" s="9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="AH63" s="9" t="s">
+        <v>572</v>
+      </c>
+      <c r="AI63" s="9" t="s">
         <v>573</v>
-      </c>
-      <c r="AI63" s="9" t="s">
-        <v>574</v>
       </c>
       <c r="AJ63" s="9" t="s">
         <v>190</v>
@@ -10909,7 +10908,7 @@
         <v>97</v>
       </c>
       <c r="AP63" s="9" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="AQ63" s="9" t="s">
         <v>190</v>
@@ -10926,10 +10925,10 @@
         <v>46034.4274253357</v>
       </c>
       <c r="D64" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="E64" s="9" t="s">
         <v>594</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>595</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>545</v>
@@ -10944,91 +10943,91 @@
         <v>103</v>
       </c>
       <c r="J64" s="9" t="s">
+        <v>595</v>
+      </c>
+      <c r="K64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="L64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="M64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="O64" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="P64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="R64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="S64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="T64" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="U64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="W64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="X64" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA64" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AD64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AE64" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF64" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG64" s="9" t="s">
         <v>596</v>
-      </c>
-      <c r="K64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="L64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="M64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="N64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="O64" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="R64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="S64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="T64" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="U64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="V64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="W64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="X64" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AA64" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AD64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE64" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF64" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG64" s="9" t="s">
-        <v>597</v>
       </c>
       <c r="AH64" s="9" t="s">
         <v>470</v>
       </c>
       <c r="AI64" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="AJ64" s="9" t="s">
         <v>598</v>
-      </c>
-      <c r="AJ64" s="9" t="s">
-        <v>599</v>
       </c>
       <c r="AK64" s="9" t="s">
         <v>345</v>
       </c>
       <c r="AL64" s="9" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="AM64" s="9" t="s">
         <v>95</v>
@@ -11040,7 +11039,7 @@
         <v>97</v>
       </c>
       <c r="AP64" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="AQ64" s="9" t="s">
         <v>345</v>
@@ -11060,10 +11059,10 @@
         <v>346</v>
       </c>
       <c r="E65" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="F65" s="9" t="s">
         <v>602</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>603</v>
       </c>
       <c r="G65" s="9" t="s">
         <v>147</v>
@@ -11075,91 +11074,91 @@
         <v>103</v>
       </c>
       <c r="J65" s="9" t="s">
+        <v>603</v>
+      </c>
+      <c r="K65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="L65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="M65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="N65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="O65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="R65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="S65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="T65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="U65" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="V65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="W65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="X65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF65" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG65" s="9" t="s">
         <v>604</v>
       </c>
-      <c r="K65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="L65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="M65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="N65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="O65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="P65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="R65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="S65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="T65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="U65" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="V65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="W65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="X65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF65" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AG65" s="9" t="s">
+      <c r="AH65" s="9" t="s">
         <v>605</v>
       </c>
-      <c r="AH65" s="9" t="s">
+      <c r="AI65" s="9" t="s">
         <v>606</v>
       </c>
-      <c r="AI65" s="9" t="s">
+      <c r="AJ65" s="9" t="s">
         <v>607</v>
       </c>
-      <c r="AJ65" s="9" t="s">
+      <c r="AK65" s="9" t="s">
         <v>608</v>
       </c>
-      <c r="AK65" s="9" t="s">
+      <c r="AL65" s="9" t="s">
         <v>609</v>
-      </c>
-      <c r="AL65" s="9" t="s">
-        <v>610</v>
       </c>
       <c r="AM65" s="9" t="s">
         <v>95</v>
@@ -11171,10 +11170,10 @@
         <v>97</v>
       </c>
       <c r="AP65" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="AQ65" s="9" t="s">
         <v>611</v>
-      </c>
-      <c r="AQ65" s="9" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11191,7 +11190,7 @@
         <v>346</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>146</v>
@@ -11206,106 +11205,106 @@
         <v>118</v>
       </c>
       <c r="J66" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="K66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="M66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="N66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="O66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="P66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="R66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="S66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="T66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="U66" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="V66" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="W66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="X66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB66" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE66" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF66" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG66" s="9" t="s">
         <v>614</v>
       </c>
-      <c r="K66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="M66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="N66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="O66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="P66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="R66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="S66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="T66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="U66" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="V66" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="W66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="X66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AA66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AB66" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD66" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE66" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF66" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG66" s="9" t="s">
+      <c r="AH66" s="9" t="s">
         <v>615</v>
       </c>
-      <c r="AH66" s="9" t="s">
+      <c r="AI66" s="9" t="s">
         <v>616</v>
       </c>
-      <c r="AI66" s="9" t="s">
+      <c r="AJ66" s="9" t="s">
         <v>617</v>
-      </c>
-      <c r="AJ66" s="9" t="s">
-        <v>618</v>
       </c>
       <c r="AK66" s="9" t="s">
         <v>125</v>
       </c>
       <c r="AL66" s="9" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="AM66" s="9" t="s">
         <v>95</v>
       </c>
       <c r="AN66" s="9" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="AO66" s="9" t="s">
         <v>97</v>
       </c>
       <c r="AP66" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="AQ66" s="9" t="s">
         <v>621</v>
-      </c>
-      <c r="AQ66" s="9" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11319,10 +11318,10 @@
         <v>46034.4322449653</v>
       </c>
       <c r="D67" s="9" t="s">
+        <v>622</v>
+      </c>
+      <c r="E67" s="9" t="s">
         <v>623</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>624</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>545</v>
@@ -11337,7 +11336,7 @@
         <v>103</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="K67" s="9" t="s">
         <v>149</v>
@@ -11412,16 +11411,16 @@
         <v>470</v>
       </c>
       <c r="AI67" s="9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="AJ67" s="9" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="AK67" s="9" t="s">
         <v>345</v>
       </c>
       <c r="AL67" s="9" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="AM67" s="9" t="s">
         <v>95</v>
@@ -11433,7 +11432,7 @@
         <v>97</v>
       </c>
       <c r="AP67" s="9" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="AQ67" s="9" t="s">
         <v>212</v>
@@ -11453,7 +11452,7 @@
         <v>114</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>146</v>
@@ -11468,79 +11467,79 @@
         <v>103</v>
       </c>
       <c r="J68" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="K68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="L68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="M68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="N68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="O68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="P68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="R68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="S68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="T68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="U68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="V68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="W68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="X68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC68" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AF68" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AG68" s="9" t="s">
         <v>629</v>
       </c>
-      <c r="K68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="M68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="N68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="O68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="P68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="R68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="S68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="T68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="U68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="V68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="W68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="X68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="Y68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AB68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC68" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AE68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AF68" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG68" s="9" t="s">
+      <c r="AH68" s="9" t="s">
         <v>630</v>
-      </c>
-      <c r="AH68" s="9" t="s">
-        <v>631</v>
       </c>
       <c r="AI68" s="9" t="s">
         <v>212</v>
@@ -11552,7 +11551,7 @@
         <v>93</v>
       </c>
       <c r="AL68" s="9" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="AM68" s="9" t="s">
         <v>95</v>
@@ -11581,10 +11580,10 @@
         <v>46035.2949040625</v>
       </c>
       <c r="D69" s="9" t="s">
+        <v>632</v>
+      </c>
+      <c r="E69" s="9" t="s">
         <v>633</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>634</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>506</v>
@@ -11599,91 +11598,91 @@
         <v>185</v>
       </c>
       <c r="J69" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="K69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="M69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="N69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="O69" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="P69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="R69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="S69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="T69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="U69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="V69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="W69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="X69" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y69" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB69" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF69" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG69" s="9" t="s">
         <v>635</v>
       </c>
-      <c r="K69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="L69" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="M69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="N69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="O69" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="P69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="R69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="S69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="T69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="U69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="V69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="W69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="X69" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y69" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB69" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF69" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG69" s="9" t="s">
+      <c r="AH69" s="9" t="s">
         <v>636</v>
       </c>
-      <c r="AH69" s="9" t="s">
+      <c r="AI69" s="9" t="s">
         <v>637</v>
       </c>
-      <c r="AI69" s="9" t="s">
+      <c r="AJ69" s="9" t="s">
         <v>638</v>
       </c>
-      <c r="AJ69" s="9" t="s">
+      <c r="AK69" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="AK69" s="9" t="s">
+      <c r="AL69" s="9" t="s">
         <v>640</v>
-      </c>
-      <c r="AL69" s="9" t="s">
-        <v>641</v>
       </c>
       <c r="AM69" s="9" t="s">
         <v>95</v>
@@ -11695,7 +11694,7 @@
         <v>169</v>
       </c>
       <c r="AP69" s="9" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AQ69" s="9" t="s">
         <v>95</v>
@@ -11712,10 +11711,10 @@
         <v>46035.2976030324</v>
       </c>
       <c r="D70" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>643</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>644</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>360</v>
@@ -11814,7 +11813,7 @@
         <v>284</v>
       </c>
       <c r="AL70" s="9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AM70" s="9" t="s">
         <v>95</v>
@@ -11826,7 +11825,7 @@
         <v>97</v>
       </c>
       <c r="AP70" s="9" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AQ70" s="9" t="s">
         <v>364</v>
@@ -11846,7 +11845,7 @@
         <v>326</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>146</v>
@@ -11939,7 +11938,7 @@
         <v>330</v>
       </c>
       <c r="AJ71" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AK71" s="9" t="s">
         <v>332</v>
@@ -11977,7 +11976,7 @@
         <v>326</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>146</v>
@@ -12070,10 +12069,10 @@
         <v>330</v>
       </c>
       <c r="AJ72" s="9" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="AK72" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="AL72" s="9" t="s">
         <v>492</v>
@@ -12088,7 +12087,7 @@
         <v>142</v>
       </c>
       <c r="AP72" s="9" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="AQ72" s="9" t="s">
         <v>153</v>
@@ -12105,10 +12104,10 @@
         <v>46035.3033662616</v>
       </c>
       <c r="D73" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="E73" s="9" t="s">
         <v>651</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>652</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>146</v>
@@ -12219,7 +12218,7 @@
         <v>97</v>
       </c>
       <c r="AP73" s="9" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AQ73" s="9" t="s">
         <v>364</v>
@@ -12236,13 +12235,13 @@
         <v>46035.3068013426</v>
       </c>
       <c r="D74" s="9" t="s">
+        <v>653</v>
+      </c>
+      <c r="E74" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="F74" s="9" t="s">
         <v>655</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>656</v>
       </c>
       <c r="G74" s="9" t="s">
         <v>85</v>
@@ -12254,85 +12253,85 @@
         <v>103</v>
       </c>
       <c r="J74" s="9" t="s">
+        <v>656</v>
+      </c>
+      <c r="K74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="L74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="N74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="O74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="P74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="R74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="S74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="T74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="U74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="V74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="W74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="X74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD74" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF74" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AG74" s="9" t="s">
         <v>657</v>
       </c>
-      <c r="K74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="L74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="M74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="N74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="O74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="R74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="S74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="T74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="U74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="V74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="W74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="X74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD74" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF74" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG74" s="9" t="s">
+      <c r="AH74" s="9" t="s">
         <v>658</v>
       </c>
-      <c r="AH74" s="9" t="s">
+      <c r="AI74" s="9" t="s">
         <v>659</v>
       </c>
-      <c r="AI74" s="9" t="s">
+      <c r="AJ74" s="9" t="s">
         <v>660</v>
-      </c>
-      <c r="AJ74" s="9" t="s">
-        <v>661</v>
       </c>
       <c r="AK74" s="9" t="s">
         <v>111</v>
@@ -12350,7 +12349,7 @@
         <v>169</v>
       </c>
       <c r="AP74" s="9" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AQ74" s="9" t="s">
         <v>111</v>
@@ -12367,10 +12366,10 @@
         <v>46035.3075904398</v>
       </c>
       <c r="D75" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="E75" s="9" t="s">
         <v>663</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>664</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>146</v>
@@ -12481,7 +12480,7 @@
         <v>97</v>
       </c>
       <c r="AP75" s="9" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AQ75" s="9" t="s">
         <v>364</v>
@@ -12498,10 +12497,10 @@
         <v>46035.3086607292</v>
       </c>
       <c r="D76" s="9" t="s">
+        <v>665</v>
+      </c>
+      <c r="E76" s="9" t="s">
         <v>666</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>667</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>186</v>
@@ -12585,19 +12584,19 @@
         <v>106</v>
       </c>
       <c r="AG76" s="9" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="AH76" s="9" t="s">
         <v>392</v>
       </c>
       <c r="AI76" s="9" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AJ76" s="9" t="s">
         <v>423</v>
       </c>
       <c r="AK76" s="9" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="AL76" s="9" t="s">
         <v>425</v>
@@ -12615,7 +12614,7 @@
         <v>267</v>
       </c>
       <c r="AQ76" s="9" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12629,10 +12628,10 @@
         <v>46035.3109386458</v>
       </c>
       <c r="D77" s="9" t="s">
+        <v>671</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>672</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>673</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>367</v>
@@ -12647,91 +12646,91 @@
         <v>185</v>
       </c>
       <c r="J77" s="9" t="s">
+        <v>673</v>
+      </c>
+      <c r="K77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="L77" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="M77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="N77" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="O77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="P77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="R77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="S77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="T77" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="U77" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="V77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="W77" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="X77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB77" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF77" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG77" s="9" t="s">
         <v>674</v>
       </c>
-      <c r="K77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="L77" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="M77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="N77" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="O77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="R77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="S77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="T77" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="U77" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="V77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="W77" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="X77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AB77" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF77" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG77" s="9" t="s">
+      <c r="AH77" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="AH77" s="9" t="s">
+      <c r="AI77" s="10" t="s">
         <v>676</v>
       </c>
-      <c r="AI77" s="10" t="s">
+      <c r="AJ77" s="9" t="s">
         <v>677</v>
       </c>
-      <c r="AJ77" s="9" t="s">
+      <c r="AK77" s="9" t="s">
+        <v>639</v>
+      </c>
+      <c r="AL77" s="10" t="s">
         <v>678</v>
-      </c>
-      <c r="AK77" s="9" t="s">
-        <v>640</v>
-      </c>
-      <c r="AL77" s="10" t="s">
-        <v>679</v>
       </c>
       <c r="AM77" s="9" t="s">
         <v>95</v>
@@ -12743,7 +12742,7 @@
         <v>169</v>
       </c>
       <c r="AP77" s="9" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="AQ77" s="9" t="s">
         <v>95</v>
@@ -12760,10 +12759,10 @@
         <v>46035.313218287</v>
       </c>
       <c r="D78" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="E78" s="9" t="s">
         <v>681</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>682</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>421</v>
@@ -12847,19 +12846,19 @@
         <v>105</v>
       </c>
       <c r="AG78" s="9" t="s">
+        <v>682</v>
+      </c>
+      <c r="AH78" s="9" t="s">
         <v>683</v>
       </c>
-      <c r="AH78" s="9" t="s">
-        <v>684</v>
-      </c>
       <c r="AI78" s="9" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AJ78" s="9" t="s">
         <v>423</v>
       </c>
       <c r="AK78" s="9" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AL78" s="9" t="s">
         <v>425</v>
@@ -12877,7 +12876,7 @@
         <v>376</v>
       </c>
       <c r="AQ78" s="9" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12891,10 +12890,10 @@
         <v>46035.3193091319</v>
       </c>
       <c r="D79" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="E79" s="9" t="s">
         <v>687</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>688</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>186</v>
@@ -12978,19 +12977,19 @@
         <v>106</v>
       </c>
       <c r="AG79" s="9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="AH79" s="9" t="s">
         <v>392</v>
       </c>
       <c r="AI79" s="9" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="AJ79" s="9" t="s">
+        <v>689</v>
+      </c>
+      <c r="AK79" s="9" t="s">
         <v>690</v>
-      </c>
-      <c r="AK79" s="9" t="s">
-        <v>691</v>
       </c>
       <c r="AL79" s="9" t="s">
         <v>425</v>
@@ -13005,10 +13004,10 @@
         <v>97</v>
       </c>
       <c r="AP79" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="AQ79" s="9" t="s">
         <v>692</v>
-      </c>
-      <c r="AQ79" s="9" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13022,10 +13021,10 @@
         <v>46035.3288586111</v>
       </c>
       <c r="D80" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="E80" s="9" t="s">
         <v>694</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>695</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>506</v>
@@ -13040,91 +13039,91 @@
         <v>185</v>
       </c>
       <c r="J80" s="10" t="s">
+        <v>695</v>
+      </c>
+      <c r="K80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="L80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="N80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="O80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="P80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="R80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="S80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="T80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="U80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="V80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="W80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="X80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD80" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF80" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG80" s="9" t="s">
         <v>696</v>
       </c>
-      <c r="K80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="L80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="M80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="N80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="O80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="P80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="R80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="S80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="T80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="U80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="V80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="W80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="X80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="Y80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="Z80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AB80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AD80" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AF80" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG80" s="9" t="s">
+      <c r="AH80" s="10" t="s">
         <v>697</v>
       </c>
-      <c r="AH80" s="10" t="s">
+      <c r="AI80" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="AI80" s="9" t="s">
+      <c r="AJ80" s="9" t="s">
         <v>699</v>
-      </c>
-      <c r="AJ80" s="9" t="s">
-        <v>700</v>
       </c>
       <c r="AK80" s="9" t="s">
         <v>512</v>
       </c>
       <c r="AL80" s="10" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="AM80" s="9" t="s">
         <v>95</v>
@@ -13136,7 +13135,7 @@
         <v>169</v>
       </c>
       <c r="AP80" s="9" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AQ80" s="9" t="s">
         <v>95</v>

</xml_diff>